<commit_message>
Support levels, parallels and nested levels.
</commit_message>
<xml_diff>
--- a/TestExcel/Test.xlsx
+++ b/TestExcel/Test.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
   <si>
     <t>Name</t>
   </si>
@@ -78,6 +78,39 @@
   </si>
   <si>
     <t>Nullable</t>
+  </si>
+  <si>
+    <t>LVL</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>AddressId</t>
+  </si>
+  <si>
+    <t>AddressName</t>
+  </si>
+  <si>
+    <t>Properties</t>
+  </si>
+  <si>
+    <t>PropertyId</t>
+  </si>
+  <si>
+    <t>PropertyName</t>
+  </si>
+  <si>
+    <t>AutoNumber</t>
+  </si>
+  <si>
+    <t>Features</t>
+  </si>
+  <si>
+    <t>FeatureId</t>
+  </si>
+  <si>
+    <t>FeatureName</t>
   </si>
 </sst>
 </file>
@@ -101,12 +134,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -121,9 +160,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,19 +445,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.7109375" customWidth="1"/>
     <col min="2" max="2" width="25.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -424,7 +466,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -432,7 +474,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -451,8 +493,11 @@
       <c r="F4" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -468,8 +513,11 @@
       <c r="E5">
         <v>8.1999999999999993</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -483,7 +531,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -492,6 +540,122 @@
       </c>
       <c r="D7" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1</v>
+      </c>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="3">
+        <v>2</v>
+      </c>
+      <c r="E11" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="3">
+        <v>3</v>
+      </c>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- There is only one column for Type, Length, Decimals and Symbol. All basic types are supported now.
- Same syntax as Transaction editor is now supported. There is no need for Type column anymore. Samples: Num(8.2), Numeric(8.2) , DateTime, Numeric(4-), Character(20), Char(20), VarChar(300), Numeric(7.2-), etc

- ContinueOnErrors setting to allow continue even there are processing errors.

- Directory setting to allow scan for all xlsx files in a Directory.

- Support for Domain Column
  When a Domain is specified the attribute get based on this Domain. The Type column can be empty or if it has a value it specify the Domain Type.

- Improved error messages
- Allow to specify the value to look for PKValue and NullableValue
- Add Unit Testing for set data type and reading several files.
</commit_message>
<xml_diff>
--- a/TestExcel/Test.xlsx
+++ b/TestExcel/Test.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="TransactionDefinitionSheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
   <si>
     <t>Name</t>
   </si>
@@ -111,6 +111,12 @@
   </si>
   <si>
     <t>FeatureName</t>
+  </si>
+  <si>
+    <t>Level Id</t>
+  </si>
+  <si>
+    <t>Parent Id</t>
   </si>
 </sst>
 </file>
@@ -445,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,7 +464,7 @@
     <col min="7" max="7" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -466,7 +472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -474,7 +480,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -496,8 +502,14 @@
       <c r="G4" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -517,7 +529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -531,7 +543,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -542,7 +554,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>19</v>
       </c>
@@ -550,12 +562,13 @@
       <c r="C8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="H8">
         <v>1</v>
       </c>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -569,7 +582,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -580,7 +593,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
@@ -588,14 +601,16 @@
       <c r="C11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="H11">
         <v>2</v>
       </c>
-      <c r="E11" s="3">
+      <c r="I11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -609,7 +624,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -620,7 +635,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
@@ -628,12 +643,13 @@
       <c r="C14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="H14">
         <v>3</v>
       </c>
-      <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -647,7 +663,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>28</v>
       </c>

</xml_diff>